<commit_message>
Added fix for non UTF-8 characters, substitutes a '?' Added feature to only list qos path violations if change is before final hop Updated README file with correct download URLs & more Included run_in_idle.bat file
</commit_message>
<xml_diff>
--- a/create_paths.xlsx
+++ b/create_paths.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19440" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="create_paths" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>Double</t>
   </si>
   <si>
-    <t>NYC &lt;-&gt; AppNeta</t>
-  </si>
-  <si>
     <t>NYC to AppNetna</t>
   </si>
   <si>
@@ -110,13 +107,16 @@
   </si>
   <si>
     <t>Polycom Custom Solution Network</t>
+  </si>
+  <si>
+    <t>NYC &lt;-&gt; São Paulo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +129,14 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -163,16 +171,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +505,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -522,15 +535,15 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -557,15 +570,15 @@
         <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -592,21 +605,21 @@
         <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -615,23 +628,26 @@
         <v>21</v>
       </c>
       <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Partial update to support AppNeta API V3 and to support Python V3, more AppNeta API V3 changes to come.
</commit_message>
<xml_diff>
--- a/create_paths.xlsx
+++ b/create_paths.xlsx
@@ -653,4 +653,189 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7A0D706B1A5364E99F58ADD181D2C5A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c6cebdaac71416cd428be50898ad690">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9f4934e5-bf5b-444a-b4fd-4e1508039a19" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4fb442bbbd02c78ce23af8b973a875ca" ns2:_="">
+    <xsd:import namespace="9f4934e5-bf5b-444a-b4fd-4e1508039a19"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9f4934e5-bf5b-444a-b4fd-4e1508039a19" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D2695CB-4A4B-42E0-A0F2-663DA78FE4D7}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E59DC2-108A-4AE3-AA48-AF98107B7214}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F3BCDEF-C445-4C23-BCC1-DD420A8EC6C2}"/>
 </file>
</xml_diff>